<commit_message>
Etapa 3: retocar detalles menores en los notebooks de etapa 2 y avance con el notebook de etapa3 haciendo los merge, agregando las variables adicionales y aciendo las correlaciones
</commit_message>
<xml_diff>
--- a/3 - Paises Idioma español oficial/paises_hispanohablantes.xlsx
+++ b/3 - Paises Idioma español oficial/paises_hispanohablantes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian De Andrade\Desktop\Data Science\Tesis Proyecto\Datasets Final - Seleccion\3 - Paises Idioma español oficial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian De Andrade\Desktop\Data Science\Tesis Proyecto\github\IFM_TMF\3 - Paises Idioma español oficial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8865644C-CC57-4C81-940A-D4370670618B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1189C418-EABA-452D-8AD0-80B928AD273E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{562A4EFE-A30A-4497-B2FB-BF0B23E367AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{562A4EFE-A30A-4497-B2FB-BF0B23E367AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Pais</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>España</t>
   </si>
@@ -104,10 +101,79 @@
     <t>Guinea Ecuatorial</t>
   </si>
   <si>
-    <t>Español idioma oficial o gran presencia</t>
-  </si>
-  <si>
     <t>México</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Country code</t>
+  </si>
+  <si>
+    <t>Spanish language</t>
+  </si>
+  <si>
+    <t>ARG</t>
+  </si>
+  <si>
+    <t>BOL</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>CUB</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t>ESP</t>
+  </si>
+  <si>
+    <t>NIC</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>PER</t>
+  </si>
+  <si>
+    <t>VEN</t>
+  </si>
+  <si>
+    <t>CHL</t>
+  </si>
+  <si>
+    <t>CRI</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>SLV</t>
+  </si>
+  <si>
+    <t>GTM</t>
+  </si>
+  <si>
+    <t>GNQ</t>
+  </si>
+  <si>
+    <t>HND</t>
+  </si>
+  <si>
+    <t>MEX</t>
+  </si>
+  <si>
+    <t>PRY</t>
+  </si>
+  <si>
+    <t>DOM</t>
+  </si>
+  <si>
+    <t>URY</t>
   </si>
 </sst>
 </file>
@@ -479,200 +545,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7480E8A-F3F3-43E2-8CFD-AB8A481781FF}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="1" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>9</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22">
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B22" xr:uid="{A7480E8A-F3F3-43E2-8CFD-AB8A481781FF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B22">
-      <sortCondition ref="A1:A22"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>